<commit_message>
Cover my part of the job, creating Test Cases to all 5 US's from the beggining of the backlog
</commit_message>
<xml_diff>
--- a/documentation/UserStories.xlsx
+++ b/documentation/UserStories.xlsx
@@ -4,19 +4,22 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="36" windowWidth="22980" windowHeight="9552" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="36" windowWidth="22980" windowHeight="9552" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Legenda" sheetId="1" r:id="rId1"/>
     <sheet name="S1" sheetId="2" r:id="rId2"/>
-    <sheet name="Arkusz3" sheetId="3" r:id="rId3"/>
+    <sheet name="S2" sheetId="3" r:id="rId3"/>
+    <sheet name="S3" sheetId="4" r:id="rId4"/>
+    <sheet name="S4" sheetId="5" r:id="rId5"/>
+    <sheet name="S5b" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="53">
   <si>
     <t>Please use following notation for naming sheets:</t>
   </si>
@@ -94,6 +97,108 @@
   </si>
   <si>
     <t>just copy/paste it and do your work</t>
+  </si>
+  <si>
+    <t>As a user, from LS, I want to enter an account creation screen. (ACS)</t>
+  </si>
+  <si>
+    <t>Create account creation screen based on the view template</t>
+  </si>
+  <si>
+    <t>Add 'switch to ACS' behavior to the button in login screen (LS)</t>
+  </si>
+  <si>
+    <t>Create forms for e-mail and password x2</t>
+  </si>
+  <si>
+    <t>Add basic validation to created forms</t>
+  </si>
+  <si>
+    <t>Cover basic rest communication based on registration forms</t>
+  </si>
+  <si>
+    <t>From LS, check if there are no errors, while switching to ACS</t>
+  </si>
+  <si>
+    <t>Verify if button to 'switch to ACS' behaves correctly</t>
+  </si>
+  <si>
+    <t>Verify if forms are viewed properly and are accesible</t>
+  </si>
+  <si>
+    <t>Test basic verification added to forms with e.g: boundaries, wrong input, etc</t>
+  </si>
+  <si>
+    <t>Test mocked/dummy rest interface with statuses 2xx, 4xx, 5xx, and several modifications of JSON</t>
+  </si>
+  <si>
+    <t>As a user, in ACS, I want to create a new account.</t>
+  </si>
+  <si>
+    <t>Implement actual communication to the backend, with registering new account</t>
+  </si>
+  <si>
+    <t>Implement actual communication with frontend, based on retrieved data</t>
+  </si>
+  <si>
+    <t>Add 'Submit' button to send data to server</t>
+  </si>
+  <si>
+    <t>Implement verification of the data in server side of application</t>
+  </si>
+  <si>
+    <t>Cover e-mail validation link</t>
+  </si>
+  <si>
+    <t>Check if addresses are correct (REST) and JSON data is consistent</t>
+  </si>
+  <si>
+    <t>Verify if 'Submit' button behaves correctly</t>
+  </si>
+  <si>
+    <t>Verify if boundary input along with wrong input is not able to be saved</t>
+  </si>
+  <si>
+    <t>Check if clicking validation link in e-mail behaves correctly</t>
+  </si>
+  <si>
+    <t>As a user, in LS, I want to log in and access game menu. (GM)</t>
+  </si>
+  <si>
+    <t>Create game menu view based on view template</t>
+  </si>
+  <si>
+    <t>Validate logging in user</t>
+  </si>
+  <si>
+    <t>Add dummy buttons to GM</t>
+  </si>
+  <si>
+    <t>Check if GM is viewed correctly</t>
+  </si>
+  <si>
+    <t>Check if 'Log in' button behaves correctly and switches view to GM</t>
+  </si>
+  <si>
+    <t>Verify if boundary input along with wrong input forbids a user to log in</t>
+  </si>
+  <si>
+    <t>Check if buttons are viewed correctly and they are accessible</t>
+  </si>
+  <si>
+    <t>As a user, in GM, I want to have following buttons/functionalities: New Game</t>
+  </si>
+  <si>
+    <t>Implement correct behavior (switch to GAMEPLAY screen) to 'New Game' button in GM</t>
+  </si>
+  <si>
+    <t>Create dummy GAMEPLAY screen view</t>
+  </si>
+  <si>
+    <t>Check if after clicking 'New Game' it actually switches to GAMEPLAY dummy screen</t>
+  </si>
+  <si>
+    <t>Check if 'New Game' button is accesible and does not generate any error when clicked</t>
   </si>
 </sst>
 </file>
@@ -198,7 +303,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -217,6 +322,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -563,8 +674,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -741,12 +852,717 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B2:E25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="81.44140625" customWidth="1"/>
+    <col min="5" max="5" width="77.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="E2" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="E3" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B5" s="4">
+        <v>1</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B6" s="4">
+        <v>2</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B7" s="4">
+        <v>3</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B8" s="4">
+        <v>4</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B9" s="4">
+        <v>5</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B10" s="4">
+        <v>6</v>
+      </c>
+      <c r="C10" s="8"/>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B11" s="4">
+        <v>7</v>
+      </c>
+      <c r="C11" s="8"/>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B12" s="4">
+        <v>8</v>
+      </c>
+      <c r="C12" s="8"/>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B13" s="4">
+        <v>9</v>
+      </c>
+      <c r="C13" s="8"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B14" s="4">
+        <v>10</v>
+      </c>
+      <c r="C14" s="8"/>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B15" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="6"/>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B16" s="5">
+        <v>1</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B17" s="5">
+        <v>2</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B18" s="5">
+        <v>3</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B19" s="5">
+        <v>4</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B20" s="5">
+        <v>5</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B21" s="5">
+        <v>6</v>
+      </c>
+      <c r="C21" s="7"/>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B22" s="5">
+        <v>7</v>
+      </c>
+      <c r="C22" s="7"/>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B23" s="5">
+        <v>8</v>
+      </c>
+      <c r="C23" s="7"/>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B24" s="5">
+        <v>9</v>
+      </c>
+      <c r="C24" s="7"/>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B25" s="5">
+        <v>10</v>
+      </c>
+      <c r="C25" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:E25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E19" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="81.44140625" customWidth="1"/>
+    <col min="5" max="5" width="77.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="E2" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="E3" s="12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B5" s="4">
+        <v>1</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B6" s="4">
+        <v>2</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B7" s="4">
+        <v>3</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B8" s="4">
+        <v>4</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B9" s="4">
+        <v>5</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B10" s="4">
+        <v>6</v>
+      </c>
+      <c r="C10" s="8"/>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B11" s="4">
+        <v>7</v>
+      </c>
+      <c r="C11" s="8"/>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B12" s="4">
+        <v>8</v>
+      </c>
+      <c r="C12" s="8"/>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B13" s="4">
+        <v>9</v>
+      </c>
+      <c r="C13" s="8"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B14" s="4">
+        <v>10</v>
+      </c>
+      <c r="C14" s="8"/>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B15" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="6"/>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B16" s="5">
+        <v>1</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B17" s="5">
+        <v>2</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B18" s="5">
+        <v>3</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B19" s="5">
+        <v>4</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B20" s="5">
+        <v>5</v>
+      </c>
+      <c r="C20" s="7"/>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B21" s="5">
+        <v>6</v>
+      </c>
+      <c r="C21" s="7"/>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B22" s="5">
+        <v>7</v>
+      </c>
+      <c r="C22" s="7"/>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B23" s="5">
+        <v>8</v>
+      </c>
+      <c r="C23" s="7"/>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B24" s="5">
+        <v>9</v>
+      </c>
+      <c r="C24" s="7"/>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B25" s="5">
+        <v>10</v>
+      </c>
+      <c r="C25" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:E25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C26" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="81.44140625" customWidth="1"/>
+    <col min="5" max="5" width="77.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="E2" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="E3" s="12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B5" s="4">
+        <v>1</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B6" s="4">
+        <v>2</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B7" s="4">
+        <v>3</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B8" s="4">
+        <v>4</v>
+      </c>
+      <c r="C8" s="8"/>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B9" s="4">
+        <v>5</v>
+      </c>
+      <c r="C9" s="8"/>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B10" s="4">
+        <v>6</v>
+      </c>
+      <c r="C10" s="8"/>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B11" s="4">
+        <v>7</v>
+      </c>
+      <c r="C11" s="8"/>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B12" s="4">
+        <v>8</v>
+      </c>
+      <c r="C12" s="8"/>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B13" s="4">
+        <v>9</v>
+      </c>
+      <c r="C13" s="8"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B14" s="4">
+        <v>10</v>
+      </c>
+      <c r="C14" s="8"/>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B15" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="6"/>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B16" s="5">
+        <v>1</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B17" s="5">
+        <v>2</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B18" s="5">
+        <v>3</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B19" s="5">
+        <v>4</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B20" s="5">
+        <v>5</v>
+      </c>
+      <c r="C20" s="7"/>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B21" s="5">
+        <v>6</v>
+      </c>
+      <c r="C21" s="7"/>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B22" s="5">
+        <v>7</v>
+      </c>
+      <c r="C22" s="7"/>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B23" s="5">
+        <v>8</v>
+      </c>
+      <c r="C23" s="7"/>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B24" s="5">
+        <v>9</v>
+      </c>
+      <c r="C24" s="7"/>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B25" s="5">
+        <v>10</v>
+      </c>
+      <c r="C25" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:E25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="81.44140625" customWidth="1"/>
+    <col min="5" max="5" width="77.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="E2" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="E3" s="12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B5" s="4">
+        <v>1</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B6" s="4">
+        <v>2</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B7" s="4">
+        <v>3</v>
+      </c>
+      <c r="C7" s="8"/>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B8" s="4">
+        <v>4</v>
+      </c>
+      <c r="C8" s="8"/>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B9" s="4">
+        <v>5</v>
+      </c>
+      <c r="C9" s="8"/>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B10" s="4">
+        <v>6</v>
+      </c>
+      <c r="C10" s="8"/>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B11" s="4">
+        <v>7</v>
+      </c>
+      <c r="C11" s="8"/>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B12" s="4">
+        <v>8</v>
+      </c>
+      <c r="C12" s="8"/>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B13" s="4">
+        <v>9</v>
+      </c>
+      <c r="C13" s="8"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B14" s="4">
+        <v>10</v>
+      </c>
+      <c r="C14" s="8"/>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B15" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="6"/>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B16" s="5">
+        <v>1</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B17" s="5">
+        <v>2</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B18" s="5">
+        <v>3</v>
+      </c>
+      <c r="C18" s="7"/>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B19" s="5">
+        <v>4</v>
+      </c>
+      <c r="C19" s="7"/>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B20" s="5">
+        <v>5</v>
+      </c>
+      <c r="C20" s="7"/>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B21" s="5">
+        <v>6</v>
+      </c>
+      <c r="C21" s="7"/>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B22" s="5">
+        <v>7</v>
+      </c>
+      <c r="C22" s="7"/>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B23" s="5">
+        <v>8</v>
+      </c>
+      <c r="C23" s="7"/>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B24" s="5">
+        <v>9</v>
+      </c>
+      <c r="C24" s="7"/>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B25" s="5">
+        <v>10</v>
+      </c>
+      <c r="C25" s="7"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>